<commit_message>
OPH-1845 haetaan suorittajien tiedotkin tietokannasta exceliin
</commit_message>
<xml_diff>
--- a/ttk/resources/tutosat_export_base.xlsx
+++ b/ttk/resources/tutosat_export_base.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anttivi/work/projects/oph/src/aitu/ttk/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anttivi/work/projects/oph/src/aitu/ttk/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="24660" windowHeight="14440" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="24660" windowHeight="14440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Suoritukset" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="1689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="1689">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -5618,7 +5618,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C5" t="str">
-        <f>IFERROR(LOOKUP($B5,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B5,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E5" t="str">
@@ -5648,7 +5648,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C6" t="str">
-        <f>IFERROR(LOOKUP($B6,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B6,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E6" t="str">
@@ -5677,7 +5677,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C7" t="str">
-        <f>IFERROR(LOOKUP($B7,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B7,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E7" t="str">
@@ -5700,7 +5700,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C8" t="str">
-        <f>IFERROR(LOOKUP($B8,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B8,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E8" t="str">
@@ -5717,7 +5717,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C9" t="str">
-        <f>IFERROR(LOOKUP($B9,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B9,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E9" t="str">
@@ -5731,7 +5731,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C10" t="str">
-        <f>IFERROR(LOOKUP($B10,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B10,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E10" t="str">
@@ -5751,7 +5751,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C11" t="str">
-        <f>IFERROR(LOOKUP($B11,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B11,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E11" t="str">
@@ -5774,7 +5774,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C12" t="str">
-        <f>IFERROR(LOOKUP($B12,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B12,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E12" t="str">
@@ -5791,7 +5791,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C13" t="str">
-        <f>IFERROR(LOOKUP($B13,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B13,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E13" t="str">
@@ -5808,7 +5808,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C14" t="str">
-        <f>IFERROR(LOOKUP($B14,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B14,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E14" t="str">
@@ -5822,7 +5822,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C15" t="str">
-        <f>IFERROR(LOOKUP($B15,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B15,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E15" t="str">
@@ -5836,7 +5836,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C16" t="str">
-        <f>IFERROR(LOOKUP($B16,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B16,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E16" t="str">
@@ -5850,7 +5850,7 @@
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C17" t="str">
-        <f>IFERROR(LOOKUP($B17,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B17,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E17" t="str">
@@ -5867,7 +5867,7 @@
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C18" t="str">
-        <f>IFERROR(LOOKUP($B18,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B18,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E18" t="str">
@@ -5881,7 +5881,7 @@
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C19" t="str">
-        <f>IFERROR(LOOKUP($B19,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B19,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E19" t="str">
@@ -5895,7 +5895,7 @@
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C20" t="str">
-        <f>IFERROR(LOOKUP($B20,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B20,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E20" t="str">
@@ -5909,7 +5909,7 @@
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C21" t="str">
-        <f>IFERROR(LOOKUP($B21,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B21,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E21" t="str">
@@ -5923,7 +5923,7 @@
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C22" t="str">
-        <f>IFERROR(LOOKUP($B22,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B22,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E22" t="str">
@@ -5937,7 +5937,7 @@
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C23" t="str">
-        <f>IFERROR(LOOKUP($B23,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B23,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E23" t="str">
@@ -5951,7 +5951,7 @@
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C24" t="str">
-        <f>IFERROR(LOOKUP($B24,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B24,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E24" t="str">
@@ -5965,7 +5965,7 @@
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C25" t="str">
-        <f>IFERROR(LOOKUP($B25,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B25,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E25" t="str">
@@ -5979,7 +5979,7 @@
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C26" t="str">
-        <f>IFERROR(LOOKUP($B26,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B26,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E26" t="str">
@@ -5993,7 +5993,7 @@
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C27" t="str">
-        <f>IFERROR(LOOKUP($B27,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B27,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E27" t="str">
@@ -6007,7 +6007,7 @@
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C28" t="str">
-        <f>IFERROR(LOOKUP($B28,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B28,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E28" t="str">
@@ -6021,7 +6021,7 @@
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C29" t="str">
-        <f>IFERROR(LOOKUP($B29,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B29,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E29" t="str">
@@ -6035,7 +6035,7 @@
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C30" t="str">
-        <f>IFERROR(LOOKUP($B30,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B30,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E30" t="str">
@@ -6049,7 +6049,7 @@
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C31" t="str">
-        <f>IFERROR(LOOKUP($B31,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B31,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E31" t="str">
@@ -6063,7 +6063,7 @@
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C32" t="str">
-        <f>IFERROR(LOOKUP($B32,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B32,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E32" t="str">
@@ -6077,7 +6077,7 @@
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C33" t="str">
-        <f>IFERROR(LOOKUP($B33,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B33,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E33" t="str">
@@ -6091,7 +6091,7 @@
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C34" t="str">
-        <f>IFERROR(LOOKUP($B34,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B34,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E34" t="str">
@@ -6105,7 +6105,7 @@
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C35" t="str">
-        <f>IFERROR(LOOKUP($B35,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B35,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E35" t="str">
@@ -6119,7 +6119,7 @@
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C36" t="str">
-        <f>IFERROR(LOOKUP($B36,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B36,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E36" t="str">
@@ -6133,7 +6133,7 @@
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C37" t="str">
-        <f>IFERROR(LOOKUP($B37,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B37,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E37" t="str">
@@ -6147,7 +6147,7 @@
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C38" t="str">
-        <f>IFERROR(LOOKUP($B38,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B38,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E38" t="str">
@@ -6161,7 +6161,7 @@
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C39" t="str">
-        <f>IFERROR(LOOKUP($B39,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B39,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E39" t="str">
@@ -6175,7 +6175,7 @@
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C40" t="str">
-        <f>IFERROR(LOOKUP($B40,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B40,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E40" t="str">
@@ -6189,7 +6189,7 @@
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C41" t="str">
-        <f>IFERROR(LOOKUP($B41,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B41,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E41" t="str">
@@ -6203,7 +6203,7 @@
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C42" t="str">
-        <f>IFERROR(LOOKUP($B42,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B42,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E42" t="str">
@@ -6217,7 +6217,7 @@
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C43" t="str">
-        <f>IFERROR(LOOKUP($B43,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B43,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E43" t="str">
@@ -6231,7 +6231,7 @@
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C44" t="str">
-        <f>IFERROR(LOOKUP($B44,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B44,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E44" t="str">
@@ -6245,7 +6245,7 @@
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C45" t="str">
-        <f>IFERROR(LOOKUP($B45,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B45,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E45" t="str">
@@ -6259,7 +6259,7 @@
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C46" t="str">
-        <f>IFERROR(LOOKUP($B46,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B46,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E46" t="str">
@@ -6273,7 +6273,7 @@
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C47" t="str">
-        <f>IFERROR(LOOKUP($B47,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B47,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E47" t="str">
@@ -6287,7 +6287,7 @@
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C48" t="str">
-        <f>IFERROR(LOOKUP($B48,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B48,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E48" t="str">
@@ -6301,7 +6301,7 @@
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C49" t="str">
-        <f>IFERROR(LOOKUP($B49,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B49,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E49" t="str">
@@ -6315,7 +6315,7 @@
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C50" t="str">
-        <f>IFERROR(LOOKUP($B50,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B50,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E50" t="str">
@@ -6329,7 +6329,7 @@
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C51" t="str">
-        <f>IFERROR(LOOKUP($B51,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B51,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E51" t="str">
@@ -6343,7 +6343,7 @@
     </row>
     <row r="52" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C52" t="str">
-        <f>IFERROR(LOOKUP($B52,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B52,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E52" t="str">
@@ -6357,7 +6357,7 @@
     </row>
     <row r="53" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C53" t="str">
-        <f>IFERROR(LOOKUP($B53,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B53,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E53" t="str">
@@ -6371,7 +6371,7 @@
     </row>
     <row r="54" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C54" t="str">
-        <f>IFERROR(LOOKUP($B54,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B54,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E54" t="str">
@@ -6385,7 +6385,7 @@
     </row>
     <row r="55" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C55" t="str">
-        <f>IFERROR(LOOKUP($B55,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B55,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E55" t="str">
@@ -6399,7 +6399,7 @@
     </row>
     <row r="56" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C56" t="str">
-        <f>IFERROR(LOOKUP($B56,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B56,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E56" t="str">
@@ -6413,7 +6413,7 @@
     </row>
     <row r="57" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C57" t="str">
-        <f>IFERROR(LOOKUP($B57,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B57,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E57" t="str">
@@ -6427,7 +6427,7 @@
     </row>
     <row r="58" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C58" t="str">
-        <f>IFERROR(LOOKUP($B58,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B58,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E58" t="str">
@@ -6441,7 +6441,7 @@
     </row>
     <row r="59" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C59" t="str">
-        <f>IFERROR(LOOKUP($B59,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B59,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E59" t="str">
@@ -6455,7 +6455,7 @@
     </row>
     <row r="60" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C60" t="str">
-        <f>IFERROR(LOOKUP($B60,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B60,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E60" t="str">
@@ -6469,7 +6469,7 @@
     </row>
     <row r="61" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C61" t="str">
-        <f>IFERROR(LOOKUP($B61,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B61,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E61" t="str">
@@ -6483,7 +6483,7 @@
     </row>
     <row r="62" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C62" t="str">
-        <f>IFERROR(LOOKUP($B62,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B62,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E62" t="str">
@@ -6497,7 +6497,7 @@
     </row>
     <row r="63" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C63" t="str">
-        <f>IFERROR(LOOKUP($B63,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B63,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E63" t="str">
@@ -6511,7 +6511,7 @@
     </row>
     <row r="64" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C64" t="str">
-        <f>IFERROR(LOOKUP($B64,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B64,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E64" t="str">
@@ -6525,7 +6525,7 @@
     </row>
     <row r="65" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C65" t="str">
-        <f>IFERROR(LOOKUP($B65,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B65,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E65" t="str">
@@ -6539,7 +6539,7 @@
     </row>
     <row r="66" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C66" t="str">
-        <f>IFERROR(LOOKUP($B66,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B66,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E66" t="str">
@@ -6553,7 +6553,7 @@
     </row>
     <row r="67" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C67" t="str">
-        <f>IFERROR(LOOKUP($B67,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B67,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E67" t="str">
@@ -6567,7 +6567,7 @@
     </row>
     <row r="68" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C68" t="str">
-        <f>IFERROR(LOOKUP($B68,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B68,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E68" t="str">
@@ -6581,7 +6581,7 @@
     </row>
     <row r="69" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C69" t="str">
-        <f>IFERROR(LOOKUP($B69,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B69,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E69" t="str">
@@ -6595,7 +6595,7 @@
     </row>
     <row r="70" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C70" t="str">
-        <f>IFERROR(LOOKUP($B70,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B70,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E70" t="str">
@@ -6609,7 +6609,7 @@
     </row>
     <row r="71" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C71" t="str">
-        <f>IFERROR(LOOKUP($B71,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B71,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E71" t="str">
@@ -6623,7 +6623,7 @@
     </row>
     <row r="72" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C72" t="str">
-        <f>IFERROR(LOOKUP($B72,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B72,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E72" t="str">
@@ -6637,7 +6637,7 @@
     </row>
     <row r="73" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C73" t="str">
-        <f>IFERROR(LOOKUP($B73,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B73,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E73" t="str">
@@ -6651,7 +6651,7 @@
     </row>
     <row r="74" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C74" t="str">
-        <f>IFERROR(LOOKUP($B74,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B74,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E74" t="str">
@@ -6665,7 +6665,7 @@
     </row>
     <row r="75" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C75" t="str">
-        <f>IFERROR(LOOKUP($B75,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B75,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E75" t="str">
@@ -6679,7 +6679,7 @@
     </row>
     <row r="76" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C76" t="str">
-        <f>IFERROR(LOOKUP($B76,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B76,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E76" t="str">
@@ -6693,7 +6693,7 @@
     </row>
     <row r="77" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C77" t="str">
-        <f>IFERROR(LOOKUP($B77,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B77,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E77" t="str">
@@ -6707,7 +6707,7 @@
     </row>
     <row r="78" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C78" t="str">
-        <f>IFERROR(LOOKUP($B78,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B78,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E78" t="str">
@@ -6721,7 +6721,7 @@
     </row>
     <row r="79" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C79" t="str">
-        <f>IFERROR(LOOKUP($B79,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B79,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E79" t="str">
@@ -6735,7 +6735,7 @@
     </row>
     <row r="80" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C80" t="str">
-        <f>IFERROR(LOOKUP($B80,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B80,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E80" t="str">
@@ -6749,7 +6749,7 @@
     </row>
     <row r="81" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C81" t="str">
-        <f>IFERROR(LOOKUP($B81,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B81,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E81" t="str">
@@ -6763,7 +6763,7 @@
     </row>
     <row r="82" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C82" t="str">
-        <f>IFERROR(LOOKUP($B82,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B82,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E82" t="str">
@@ -6777,7 +6777,7 @@
     </row>
     <row r="83" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C83" t="str">
-        <f>IFERROR(LOOKUP($B83,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B83,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E83" t="str">
@@ -6791,7 +6791,7 @@
     </row>
     <row r="84" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C84" t="str">
-        <f>IFERROR(LOOKUP($B84,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B84,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E84" t="str">
@@ -6805,7 +6805,7 @@
     </row>
     <row r="85" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C85" t="str">
-        <f>IFERROR(LOOKUP($B85,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B85,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E85" t="str">
@@ -6819,7 +6819,7 @@
     </row>
     <row r="86" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C86" t="str">
-        <f>IFERROR(LOOKUP($B86,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B86,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E86" t="str">
@@ -6833,7 +6833,7 @@
     </row>
     <row r="87" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C87" t="str">
-        <f>IFERROR(LOOKUP($B87,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B87,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E87" t="str">
@@ -6847,7 +6847,7 @@
     </row>
     <row r="88" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C88" t="str">
-        <f>IFERROR(LOOKUP($B88,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B88,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E88" t="str">
@@ -6861,7 +6861,7 @@
     </row>
     <row r="89" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C89" t="str">
-        <f>IFERROR(LOOKUP($B89,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B89,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E89" t="str">
@@ -6875,7 +6875,7 @@
     </row>
     <row r="90" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C90" t="str">
-        <f>IFERROR(LOOKUP($B90,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B90,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E90" t="str">
@@ -6889,7 +6889,7 @@
     </row>
     <row r="91" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C91" t="str">
-        <f>IFERROR(LOOKUP($B91,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B91,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E91" t="str">
@@ -6903,7 +6903,7 @@
     </row>
     <row r="92" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C92" t="str">
-        <f>IFERROR(LOOKUP($B92,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B92,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E92" t="str">
@@ -6917,7 +6917,7 @@
     </row>
     <row r="93" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C93" t="str">
-        <f>IFERROR(LOOKUP($B93,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B93,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E93" t="str">
@@ -6931,7 +6931,7 @@
     </row>
     <row r="94" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C94" t="str">
-        <f>IFERROR(LOOKUP($B94,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B94,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E94" t="str">
@@ -6945,7 +6945,7 @@
     </row>
     <row r="95" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C95" t="str">
-        <f>IFERROR(LOOKUP($B95,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B95,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E95" t="str">
@@ -6959,7 +6959,7 @@
     </row>
     <row r="96" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C96" t="str">
-        <f>IFERROR(LOOKUP($B96,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B96,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E96" t="str">
@@ -6973,7 +6973,7 @@
     </row>
     <row r="97" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C97" t="str">
-        <f>IFERROR(LOOKUP($B97,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B97,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E97" t="str">
@@ -6987,7 +6987,7 @@
     </row>
     <row r="98" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C98" t="str">
-        <f>IFERROR(LOOKUP($B98,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B98,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E98" t="str">
@@ -7001,7 +7001,7 @@
     </row>
     <row r="99" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C99" t="str">
-        <f>IFERROR(LOOKUP($B99,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B99,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E99" t="str">
@@ -7015,7 +7015,7 @@
     </row>
     <row r="100" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C100" t="str">
-        <f>IFERROR(LOOKUP($B100,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B100,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E100" t="str">
@@ -7029,7 +7029,7 @@
     </row>
     <row r="101" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C101" t="str">
-        <f>IFERROR(LOOKUP($B101,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B101,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E101" t="str">
@@ -7043,7 +7043,7 @@
     </row>
     <row r="102" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C102" t="str">
-        <f>IFERROR(LOOKUP($B102,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B102,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E102" t="str">
@@ -7057,7 +7057,7 @@
     </row>
     <row r="103" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C103" t="str">
-        <f>IFERROR(LOOKUP($B103,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B103,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E103" t="str">
@@ -7071,7 +7071,7 @@
     </row>
     <row r="104" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C104" t="str">
-        <f>IFERROR(LOOKUP($B104,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B104,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E104" t="str">
@@ -7085,7 +7085,7 @@
     </row>
     <row r="105" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C105" t="str">
-        <f>IFERROR(LOOKUP($B105,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B105,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E105" t="str">
@@ -7099,7 +7099,7 @@
     </row>
     <row r="106" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C106" t="str">
-        <f>IFERROR(LOOKUP($B106,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B106,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E106" t="str">
@@ -7113,7 +7113,7 @@
     </row>
     <row r="107" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C107" t="str">
-        <f>IFERROR(LOOKUP($B107,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B107,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E107" t="str">
@@ -7127,7 +7127,7 @@
     </row>
     <row r="108" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C108" t="str">
-        <f>IFERROR(LOOKUP($B108,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B108,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E108" t="str">
@@ -7141,7 +7141,7 @@
     </row>
     <row r="109" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C109" t="str">
-        <f>IFERROR(LOOKUP($B109,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B109,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E109" t="str">
@@ -7155,7 +7155,7 @@
     </row>
     <row r="110" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C110" t="str">
-        <f>IFERROR(LOOKUP($B110,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B110,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E110" t="str">
@@ -7169,7 +7169,7 @@
     </row>
     <row r="111" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C111" t="str">
-        <f>IFERROR(LOOKUP($B111,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B111,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E111" t="str">
@@ -7183,7 +7183,7 @@
     </row>
     <row r="112" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C112" t="str">
-        <f>IFERROR(LOOKUP($B112,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B112,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E112" t="str">
@@ -7197,7 +7197,7 @@
     </row>
     <row r="113" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C113" t="str">
-        <f>IFERROR(LOOKUP($B113,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B113,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E113" t="str">
@@ -7211,7 +7211,7 @@
     </row>
     <row r="114" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C114" t="str">
-        <f>IFERROR(LOOKUP($B114,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B114,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E114" t="str">
@@ -7225,7 +7225,7 @@
     </row>
     <row r="115" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C115" t="str">
-        <f>IFERROR(LOOKUP($B115,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B115,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E115" t="str">
@@ -7239,7 +7239,7 @@
     </row>
     <row r="116" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C116" t="str">
-        <f>IFERROR(LOOKUP($B116,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B116,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E116" t="str">
@@ -7253,7 +7253,7 @@
     </row>
     <row r="117" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C117" t="str">
-        <f>IFERROR(LOOKUP($B117,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B117,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E117" t="str">
@@ -7267,7 +7267,7 @@
     </row>
     <row r="118" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C118" t="str">
-        <f>IFERROR(LOOKUP($B118,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B118,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E118" t="str">
@@ -7281,7 +7281,7 @@
     </row>
     <row r="119" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C119" t="str">
-        <f>IFERROR(LOOKUP($B119,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B119,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E119" t="str">
@@ -7295,7 +7295,7 @@
     </row>
     <row r="120" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C120" t="str">
-        <f>IFERROR(LOOKUP($B120,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B120,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E120" t="str">
@@ -7309,7 +7309,7 @@
     </row>
     <row r="121" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C121" t="str">
-        <f>IFERROR(LOOKUP($B121,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B121,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E121" t="str">
@@ -7323,7 +7323,7 @@
     </row>
     <row r="122" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C122" t="str">
-        <f>IFERROR(LOOKUP($B122,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B122,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E122" t="str">
@@ -7337,7 +7337,7 @@
     </row>
     <row r="123" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C123" t="str">
-        <f>IFERROR(LOOKUP($B123,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B123,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E123" t="str">
@@ -7351,7 +7351,7 @@
     </row>
     <row r="124" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C124" t="str">
-        <f>IFERROR(LOOKUP($B124,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B124,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E124" t="str">
@@ -7365,7 +7365,7 @@
     </row>
     <row r="125" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C125" t="str">
-        <f>IFERROR(LOOKUP($B125,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B125,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E125" t="str">
@@ -7379,7 +7379,7 @@
     </row>
     <row r="126" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C126" t="str">
-        <f>IFERROR(LOOKUP($B126,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B126,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E126" t="str">
@@ -7393,7 +7393,7 @@
     </row>
     <row r="127" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C127" t="str">
-        <f>IFERROR(LOOKUP($B127,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B127,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E127" t="str">
@@ -7407,7 +7407,7 @@
     </row>
     <row r="128" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C128" t="str">
-        <f>IFERROR(LOOKUP($B128,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B128,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E128" t="str">
@@ -7421,7 +7421,7 @@
     </row>
     <row r="129" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C129" t="str">
-        <f>IFERROR(LOOKUP($B129,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B129,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E129" t="str">
@@ -7435,7 +7435,7 @@
     </row>
     <row r="130" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C130" t="str">
-        <f>IFERROR(LOOKUP($B130,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B130,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E130" t="str">
@@ -7449,7 +7449,7 @@
     </row>
     <row r="131" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C131" t="str">
-        <f>IFERROR(LOOKUP($B131,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B131,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E131" t="str">
@@ -7463,7 +7463,7 @@
     </row>
     <row r="132" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C132" t="str">
-        <f>IFERROR(LOOKUP($B132,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B132,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E132" t="str">
@@ -7477,7 +7477,7 @@
     </row>
     <row r="133" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C133" t="str">
-        <f>IFERROR(LOOKUP($B133,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B133,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E133" t="str">
@@ -7491,7 +7491,7 @@
     </row>
     <row r="134" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C134" t="str">
-        <f>IFERROR(LOOKUP($B134,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B134,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E134" t="str">
@@ -7505,7 +7505,7 @@
     </row>
     <row r="135" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C135" t="str">
-        <f>IFERROR(LOOKUP($B135,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B135,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E135" t="str">
@@ -7519,7 +7519,7 @@
     </row>
     <row r="136" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C136" t="str">
-        <f>IFERROR(LOOKUP($B136,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B136,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E136" t="str">
@@ -7533,7 +7533,7 @@
     </row>
     <row r="137" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C137" t="str">
-        <f>IFERROR(LOOKUP($B137,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B137,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E137" t="str">
@@ -7547,7 +7547,7 @@
     </row>
     <row r="138" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C138" t="str">
-        <f>IFERROR(LOOKUP($B138,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B138,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E138" t="str">
@@ -7561,7 +7561,7 @@
     </row>
     <row r="139" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C139" t="str">
-        <f>IFERROR(LOOKUP($B139,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B139,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E139" t="str">
@@ -7575,7 +7575,7 @@
     </row>
     <row r="140" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C140" t="str">
-        <f>IFERROR(LOOKUP($B140,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B140,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E140" t="str">
@@ -7589,7 +7589,7 @@
     </row>
     <row r="141" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C141" t="str">
-        <f>IFERROR(LOOKUP($B141,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B141,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E141" t="str">
@@ -7603,7 +7603,7 @@
     </row>
     <row r="142" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C142" t="str">
-        <f>IFERROR(LOOKUP($B142,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B142,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E142" t="str">
@@ -7617,7 +7617,7 @@
     </row>
     <row r="143" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C143" t="str">
-        <f>IFERROR(LOOKUP($B143,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B143,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E143" t="str">
@@ -7631,7 +7631,7 @@
     </row>
     <row r="144" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C144" t="str">
-        <f>IFERROR(LOOKUP($B144,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B144,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E144" t="str">
@@ -7645,7 +7645,7 @@
     </row>
     <row r="145" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C145" t="str">
-        <f>IFERROR(LOOKUP($B145,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B145,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E145" t="str">
@@ -7659,7 +7659,7 @@
     </row>
     <row r="146" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C146" t="str">
-        <f>IFERROR(LOOKUP($B146,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B146,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E146" t="str">
@@ -7673,7 +7673,7 @@
     </row>
     <row r="147" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C147" t="str">
-        <f>IFERROR(LOOKUP($B147,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B147,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E147" t="str">
@@ -7687,7 +7687,7 @@
     </row>
     <row r="148" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C148" t="str">
-        <f>IFERROR(LOOKUP($B148,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B148,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E148" t="str">
@@ -7701,7 +7701,7 @@
     </row>
     <row r="149" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C149" t="str">
-        <f>IFERROR(LOOKUP($B149,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B149,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E149" t="str">
@@ -7715,7 +7715,7 @@
     </row>
     <row r="150" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C150" t="str">
-        <f>IFERROR(LOOKUP($B150,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B150,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E150" t="str">
@@ -7729,7 +7729,7 @@
     </row>
     <row r="151" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C151" t="str">
-        <f>IFERROR(LOOKUP($B151,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B151,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E151" t="str">
@@ -7743,7 +7743,7 @@
     </row>
     <row r="152" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C152" t="str">
-        <f>IFERROR(LOOKUP($B152,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B152,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E152" t="str">
@@ -7757,7 +7757,7 @@
     </row>
     <row r="153" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C153" t="str">
-        <f>IFERROR(LOOKUP($B153,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B153,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E153" t="str">
@@ -7771,7 +7771,7 @@
     </row>
     <row r="154" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C154" t="str">
-        <f>IFERROR(LOOKUP($B154,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B154,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E154" t="str">
@@ -7785,7 +7785,7 @@
     </row>
     <row r="155" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C155" t="str">
-        <f>IFERROR(LOOKUP($B155,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B155,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E155" t="str">
@@ -7799,7 +7799,7 @@
     </row>
     <row r="156" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C156" t="str">
-        <f>IFERROR(LOOKUP($B156,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B156,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E156" t="str">
@@ -7813,7 +7813,7 @@
     </row>
     <row r="157" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C157" t="str">
-        <f>IFERROR(LOOKUP($B157,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B157,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E157" t="str">
@@ -7827,7 +7827,7 @@
     </row>
     <row r="158" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C158" t="str">
-        <f>IFERROR(LOOKUP($B158,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B158,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E158" t="str">
@@ -7841,7 +7841,7 @@
     </row>
     <row r="159" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C159" t="str">
-        <f>IFERROR(LOOKUP($B159,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B159,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E159" t="str">
@@ -7855,7 +7855,7 @@
     </row>
     <row r="160" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C160" t="str">
-        <f>IFERROR(LOOKUP($B160,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B160,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E160" t="str">
@@ -7869,7 +7869,7 @@
     </row>
     <row r="161" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C161" t="str">
-        <f>IFERROR(LOOKUP($B161,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B161,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E161" t="str">
@@ -7883,7 +7883,7 @@
     </row>
     <row r="162" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C162" t="str">
-        <f>IFERROR(LOOKUP($B162,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B162,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E162" t="str">
@@ -7897,7 +7897,7 @@
     </row>
     <row r="163" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C163" t="str">
-        <f>IFERROR(LOOKUP($B163,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B163,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E163" t="str">
@@ -7911,7 +7911,7 @@
     </row>
     <row r="164" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C164" t="str">
-        <f>IFERROR(LOOKUP($B164,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B164,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E164" t="str">
@@ -7925,7 +7925,7 @@
     </row>
     <row r="165" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C165" t="str">
-        <f>IFERROR(LOOKUP($B165,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B165,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E165" t="str">
@@ -7939,7 +7939,7 @@
     </row>
     <row r="166" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C166" t="str">
-        <f>IFERROR(LOOKUP($B166,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B166,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E166" t="str">
@@ -7953,7 +7953,7 @@
     </row>
     <row r="167" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C167" t="str">
-        <f>IFERROR(LOOKUP($B167,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B167,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E167" t="str">
@@ -7967,7 +7967,7 @@
     </row>
     <row r="168" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C168" t="str">
-        <f>IFERROR(LOOKUP($B168,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B168,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E168" t="str">
@@ -7981,7 +7981,7 @@
     </row>
     <row r="169" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C169" t="str">
-        <f>IFERROR(LOOKUP($B169,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B169,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E169" t="str">
@@ -7995,7 +7995,7 @@
     </row>
     <row r="170" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C170" t="str">
-        <f>IFERROR(LOOKUP($B170,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B170,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E170" t="str">
@@ -8009,7 +8009,7 @@
     </row>
     <row r="171" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C171" t="str">
-        <f>IFERROR(LOOKUP($B171,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B171,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E171" t="str">
@@ -8023,7 +8023,7 @@
     </row>
     <row r="172" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C172" t="str">
-        <f>IFERROR(LOOKUP($B172,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B172,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E172" t="str">
@@ -8037,7 +8037,7 @@
     </row>
     <row r="173" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C173" t="str">
-        <f>IFERROR(LOOKUP($B173,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B173,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E173" t="str">
@@ -8051,7 +8051,7 @@
     </row>
     <row r="174" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C174" t="str">
-        <f>IFERROR(LOOKUP($B174,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B174,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E174" t="str">
@@ -8065,7 +8065,7 @@
     </row>
     <row r="175" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C175" t="str">
-        <f>IFERROR(LOOKUP($B175,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B175,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E175" t="str">
@@ -8079,7 +8079,7 @@
     </row>
     <row r="176" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C176" t="str">
-        <f>IFERROR(LOOKUP($B176,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B176,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E176" t="str">
@@ -8093,7 +8093,7 @@
     </row>
     <row r="177" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C177" t="str">
-        <f>IFERROR(LOOKUP($B177,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B177,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E177" t="str">
@@ -8107,7 +8107,7 @@
     </row>
     <row r="178" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C178" t="str">
-        <f>IFERROR(LOOKUP($B178,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B178,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E178" t="str">
@@ -8121,7 +8121,7 @@
     </row>
     <row r="179" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C179" t="str">
-        <f>IFERROR(LOOKUP($B179,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B179,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E179" t="str">
@@ -8135,7 +8135,7 @@
     </row>
     <row r="180" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C180" t="str">
-        <f>IFERROR(LOOKUP($B180,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B180,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E180" t="str">
@@ -8149,7 +8149,7 @@
     </row>
     <row r="181" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C181" t="str">
-        <f>IFERROR(LOOKUP($B181,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B181,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E181" t="str">
@@ -8163,7 +8163,7 @@
     </row>
     <row r="182" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C182" t="str">
-        <f>IFERROR(LOOKUP($B182,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B182,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E182" t="str">
@@ -8177,7 +8177,7 @@
     </row>
     <row r="183" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C183" t="str">
-        <f>IFERROR(LOOKUP($B183,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B183,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E183" t="str">
@@ -8191,7 +8191,7 @@
     </row>
     <row r="184" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C184" t="str">
-        <f>IFERROR(LOOKUP($B184,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B184,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E184" t="str">
@@ -8205,7 +8205,7 @@
     </row>
     <row r="185" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C185" t="str">
-        <f>IFERROR(LOOKUP($B185,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B185,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E185" t="str">
@@ -8219,7 +8219,7 @@
     </row>
     <row r="186" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C186" t="str">
-        <f>IFERROR(LOOKUP($B186,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B186,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E186" t="str">
@@ -8233,7 +8233,7 @@
     </row>
     <row r="187" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C187" t="str">
-        <f>IFERROR(LOOKUP($B187,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B187,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E187" t="str">
@@ -8247,7 +8247,7 @@
     </row>
     <row r="188" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C188" t="str">
-        <f>IFERROR(LOOKUP($B188,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B188,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E188" t="str">
@@ -8261,7 +8261,7 @@
     </row>
     <row r="189" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C189" t="str">
-        <f>IFERROR(LOOKUP($B189,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B189,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E189" t="str">
@@ -8275,7 +8275,7 @@
     </row>
     <row r="190" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C190" t="str">
-        <f>IFERROR(LOOKUP($B190,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B190,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E190" t="str">
@@ -8289,7 +8289,7 @@
     </row>
     <row r="191" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C191" t="str">
-        <f>IFERROR(LOOKUP($B191,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B191,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E191" t="str">
@@ -8303,7 +8303,7 @@
     </row>
     <row r="192" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C192" t="str">
-        <f>IFERROR(LOOKUP($B192,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B192,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E192" t="str">
@@ -8317,7 +8317,7 @@
     </row>
     <row r="193" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C193" t="str">
-        <f>IFERROR(LOOKUP($B193,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B193,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E193" t="str">
@@ -8331,7 +8331,7 @@
     </row>
     <row r="194" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C194" t="str">
-        <f>IFERROR(LOOKUP($B194,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B194,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E194" t="str">
@@ -8345,7 +8345,7 @@
     </row>
     <row r="195" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C195" t="str">
-        <f>IFERROR(LOOKUP($B195,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B195,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E195" t="str">
@@ -8359,7 +8359,7 @@
     </row>
     <row r="196" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C196" t="str">
-        <f>IFERROR(LOOKUP($B196,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B196,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E196" t="str">
@@ -8373,7 +8373,7 @@
     </row>
     <row r="197" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C197" t="str">
-        <f>IFERROR(LOOKUP($B197,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B197,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E197" t="str">
@@ -8387,7 +8387,7 @@
     </row>
     <row r="198" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C198" t="str">
-        <f>IFERROR(LOOKUP($B198,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B198,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E198" t="str">
@@ -8401,7 +8401,7 @@
     </row>
     <row r="199" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C199" t="str">
-        <f>IFERROR(LOOKUP($B199,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B199,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E199" t="str">
@@ -8416,7 +8416,7 @@
     <row r="200" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B200" s="14"/>
       <c r="C200" s="14" t="str">
-        <f>IFERROR(LOOKUP($B200,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B200,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="D200" s="14"/>
@@ -8438,7 +8438,7 @@
     </row>
     <row r="201" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C201" t="str">
-        <f>IFERROR(LOOKUP($B201,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B201,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E201" t="str">
@@ -8452,7 +8452,7 @@
     </row>
     <row r="202" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C202" t="str">
-        <f>IFERROR(LOOKUP($B202,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440),"")</f>
+        <f>IFERROR(LOOKUP($B202,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
         <v/>
       </c>
       <c r="E202" t="str">
@@ -8466,7 +8466,7 @@
     </row>
     <row r="203" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C203" t="str">
-        <f>IFERROR(LOOKUP($B203,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B203,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E203" t="str">
@@ -8476,7 +8476,7 @@
     </row>
     <row r="204" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C204" t="str">
-        <f>IFERROR(LOOKUP($B204,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B204,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E204" t="str">
@@ -8486,7 +8486,7 @@
     </row>
     <row r="205" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C205" t="str">
-        <f>IFERROR(LOOKUP($B205,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B205,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E205" t="str">
@@ -8496,7 +8496,7 @@
     </row>
     <row r="206" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C206" t="str">
-        <f>IFERROR(LOOKUP($B206,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B206,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E206" t="str">
@@ -8506,7 +8506,7 @@
     </row>
     <row r="207" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C207" t="str">
-        <f>IFERROR(LOOKUP($B207,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B207,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E207" t="str">
@@ -8516,7 +8516,7 @@
     </row>
     <row r="208" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C208" t="str">
-        <f>IFERROR(LOOKUP($B208,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B208,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E208" t="str">
@@ -8526,7 +8526,7 @@
     </row>
     <row r="209" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C209" t="str">
-        <f>IFERROR(LOOKUP($B209,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B209,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E209" t="str">
@@ -8536,7 +8536,7 @@
     </row>
     <row r="210" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C210" t="str">
-        <f>IFERROR(LOOKUP($B210,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B210,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E210" t="str">
@@ -8546,7 +8546,7 @@
     </row>
     <row r="211" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C211" t="str">
-        <f>IFERROR(LOOKUP($B211,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B211,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E211" t="str">
@@ -8556,7 +8556,7 @@
     </row>
     <row r="212" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C212" t="str">
-        <f>IFERROR(LOOKUP($B212,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B212,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E212" t="str">
@@ -8566,7 +8566,7 @@
     </row>
     <row r="213" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C213" t="str">
-        <f>IFERROR(LOOKUP($B213,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B213,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E213" t="str">
@@ -8576,7 +8576,7 @@
     </row>
     <row r="214" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C214" t="str">
-        <f>IFERROR(LOOKUP($B214,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B214,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E214" t="str">
@@ -8586,7 +8586,7 @@
     </row>
     <row r="215" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C215" t="str">
-        <f>IFERROR(LOOKUP($B215,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B215,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E215" t="str">
@@ -8596,7 +8596,7 @@
     </row>
     <row r="216" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C216" t="str">
-        <f>IFERROR(LOOKUP($B216,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B216,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E216" t="str">
@@ -8606,7 +8606,7 @@
     </row>
     <row r="217" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C217" t="str">
-        <f>IFERROR(LOOKUP($B217,Opiskelijat!$A$3:$A$440,Opiskelijat!$C$3:$C$440), "")</f>
+        <f>IFERROR(LOOKUP($B217,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439), "")</f>
         <v/>
       </c>
       <c r="E217" t="str">
@@ -8636,15 +8636,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Opiskelijat!$A$3:$A$21</xm:f>
+            <xm:f>tutkinnot!$A$3:$A$438</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B218</xm:sqref>
+          <xm:sqref>C219:C234 D5:D218</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>tutkinnot!$A$3:$A$438</xm:f>
+            <xm:f>Opiskelijat!$A$3:$A$20</xm:f>
           </x14:formula1>
-          <xm:sqref>C219:C234 D5:D218</xm:sqref>
+          <xm:sqref>B5:B218</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -13203,7 +13203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J438"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E438"/>
     </sheetView>
   </sheetViews>
@@ -20104,10 +20104,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D3"/>
+  <dimension ref="A2:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20126,14 +20126,6 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
OPH-1845 korjattu excelissä olevia laskukaavoja
</commit_message>
<xml_diff>
--- a/ttk/resources/tutosat_export_base.xlsx
+++ b/ttk/resources/tutosat_export_base.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="24660" windowHeight="14440" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="24660" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Suoritukset" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="1689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="1690">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -5094,6 +5094,9 @@
   </si>
   <si>
     <t>337112</t>
+  </si>
+  <si>
+    <t>suorittaja_id</t>
   </si>
 </sst>
 </file>
@@ -5498,8 +5501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P217"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K199"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5580,7 +5583,7 @@
         <v>1242</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1240</v>
+        <v>1689</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
@@ -5618,7 +5621,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C5" t="str">
-        <f>IFERROR(LOOKUP($B5,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B5,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E5" t="str">
@@ -5648,7 +5651,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C6" t="str">
-        <f>IFERROR(LOOKUP($B6,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B6,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E6" t="str">
@@ -5677,7 +5680,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C7" t="str">
-        <f>IFERROR(LOOKUP($B7,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B7,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E7" t="str">
@@ -5700,7 +5703,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C8" t="str">
-        <f>IFERROR(LOOKUP($B8,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B8,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E8" t="str">
@@ -5717,7 +5720,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C9" t="str">
-        <f>IFERROR(LOOKUP($B9,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B9,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E9" t="str">
@@ -5731,7 +5734,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C10" t="str">
-        <f>IFERROR(LOOKUP($B10,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B10,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E10" t="str">
@@ -5751,7 +5754,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C11" t="str">
-        <f>IFERROR(LOOKUP($B11,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B11,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E11" t="str">
@@ -5774,7 +5777,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C12" t="str">
-        <f>IFERROR(LOOKUP($B12,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B12,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E12" t="str">
@@ -5791,7 +5794,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C13" t="str">
-        <f>IFERROR(LOOKUP($B13,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B13,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E13" t="str">
@@ -5808,7 +5811,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C14" t="str">
-        <f>IFERROR(LOOKUP($B14,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B14,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E14" t="str">
@@ -5822,7 +5825,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C15" t="str">
-        <f>IFERROR(LOOKUP($B15,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B15,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E15" t="str">
@@ -5836,7 +5839,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C16" t="str">
-        <f>IFERROR(LOOKUP($B16,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B16,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E16" t="str">
@@ -5850,7 +5853,7 @@
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C17" t="str">
-        <f>IFERROR(LOOKUP($B17,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B17,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E17" t="str">
@@ -5867,7 +5870,7 @@
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C18" t="str">
-        <f>IFERROR(LOOKUP($B18,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B18,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E18" t="str">
@@ -5881,7 +5884,7 @@
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C19" t="str">
-        <f>IFERROR(LOOKUP($B19,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B19,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E19" t="str">
@@ -5895,7 +5898,7 @@
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C20" t="str">
-        <f>IFERROR(LOOKUP($B20,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B20,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E20" t="str">
@@ -5909,7 +5912,7 @@
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C21" t="str">
-        <f>IFERROR(LOOKUP($B21,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B21,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E21" t="str">
@@ -5923,7 +5926,7 @@
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C22" t="str">
-        <f>IFERROR(LOOKUP($B22,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B22,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E22" t="str">
@@ -5937,7 +5940,7 @@
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C23" t="str">
-        <f>IFERROR(LOOKUP($B23,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B23,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E23" t="str">
@@ -5951,7 +5954,7 @@
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C24" t="str">
-        <f>IFERROR(LOOKUP($B24,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B24,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E24" t="str">
@@ -5965,7 +5968,7 @@
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C25" t="str">
-        <f>IFERROR(LOOKUP($B25,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B25,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E25" t="str">
@@ -5979,7 +5982,7 @@
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C26" t="str">
-        <f>IFERROR(LOOKUP($B26,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B26,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E26" t="str">
@@ -5993,7 +5996,7 @@
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C27" t="str">
-        <f>IFERROR(LOOKUP($B27,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B27,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E27" t="str">
@@ -6007,7 +6010,7 @@
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C28" t="str">
-        <f>IFERROR(LOOKUP($B28,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B28,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E28" t="str">
@@ -6021,7 +6024,7 @@
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C29" t="str">
-        <f>IFERROR(LOOKUP($B29,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B29,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E29" t="str">
@@ -6035,7 +6038,7 @@
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C30" t="str">
-        <f>IFERROR(LOOKUP($B30,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B30,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E30" t="str">
@@ -6049,7 +6052,7 @@
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C31" t="str">
-        <f>IFERROR(LOOKUP($B31,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B31,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E31" t="str">
@@ -6063,7 +6066,7 @@
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C32" t="str">
-        <f>IFERROR(LOOKUP($B32,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B32,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E32" t="str">
@@ -6077,7 +6080,7 @@
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C33" t="str">
-        <f>IFERROR(LOOKUP($B33,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B33,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E33" t="str">
@@ -6091,7 +6094,7 @@
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C34" t="str">
-        <f>IFERROR(LOOKUP($B34,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B34,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E34" t="str">
@@ -6105,7 +6108,7 @@
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C35" t="str">
-        <f>IFERROR(LOOKUP($B35,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B35,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E35" t="str">
@@ -6119,7 +6122,7 @@
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C36" t="str">
-        <f>IFERROR(LOOKUP($B36,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B36,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E36" t="str">
@@ -6133,7 +6136,7 @@
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C37" t="str">
-        <f>IFERROR(LOOKUP($B37,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B37,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E37" t="str">
@@ -6147,7 +6150,7 @@
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C38" t="str">
-        <f>IFERROR(LOOKUP($B38,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B38,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E38" t="str">
@@ -6161,7 +6164,7 @@
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C39" t="str">
-        <f>IFERROR(LOOKUP($B39,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B39,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E39" t="str">
@@ -6175,7 +6178,7 @@
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C40" t="str">
-        <f>IFERROR(LOOKUP($B40,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B40,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E40" t="str">
@@ -6189,7 +6192,7 @@
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C41" t="str">
-        <f>IFERROR(LOOKUP($B41,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B41,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E41" t="str">
@@ -6203,7 +6206,7 @@
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C42" t="str">
-        <f>IFERROR(LOOKUP($B42,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B42,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E42" t="str">
@@ -6217,7 +6220,7 @@
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C43" t="str">
-        <f>IFERROR(LOOKUP($B43,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B43,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E43" t="str">
@@ -6231,7 +6234,7 @@
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C44" t="str">
-        <f>IFERROR(LOOKUP($B44,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B44,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E44" t="str">
@@ -6245,7 +6248,7 @@
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C45" t="str">
-        <f>IFERROR(LOOKUP($B45,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B45,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E45" t="str">
@@ -6259,7 +6262,7 @@
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C46" t="str">
-        <f>IFERROR(LOOKUP($B46,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B46,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E46" t="str">
@@ -6273,7 +6276,7 @@
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C47" t="str">
-        <f>IFERROR(LOOKUP($B47,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B47,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E47" t="str">
@@ -6287,7 +6290,7 @@
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C48" t="str">
-        <f>IFERROR(LOOKUP($B48,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B48,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E48" t="str">
@@ -6301,7 +6304,7 @@
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C49" t="str">
-        <f>IFERROR(LOOKUP($B49,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B49,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E49" t="str">
@@ -6315,7 +6318,7 @@
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C50" t="str">
-        <f>IFERROR(LOOKUP($B50,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B50,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E50" t="str">
@@ -6329,7 +6332,7 @@
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C51" t="str">
-        <f>IFERROR(LOOKUP($B51,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B51,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E51" t="str">
@@ -6343,7 +6346,7 @@
     </row>
     <row r="52" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C52" t="str">
-        <f>IFERROR(LOOKUP($B52,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B52,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E52" t="str">
@@ -6357,7 +6360,7 @@
     </row>
     <row r="53" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C53" t="str">
-        <f>IFERROR(LOOKUP($B53,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B53,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E53" t="str">
@@ -6371,7 +6374,7 @@
     </row>
     <row r="54" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C54" t="str">
-        <f>IFERROR(LOOKUP($B54,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B54,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E54" t="str">
@@ -6385,7 +6388,7 @@
     </row>
     <row r="55" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C55" t="str">
-        <f>IFERROR(LOOKUP($B55,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B55,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E55" t="str">
@@ -6399,7 +6402,7 @@
     </row>
     <row r="56" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C56" t="str">
-        <f>IFERROR(LOOKUP($B56,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B56,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E56" t="str">
@@ -6413,7 +6416,7 @@
     </row>
     <row r="57" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C57" t="str">
-        <f>IFERROR(LOOKUP($B57,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B57,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E57" t="str">
@@ -6427,7 +6430,7 @@
     </row>
     <row r="58" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C58" t="str">
-        <f>IFERROR(LOOKUP($B58,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B58,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E58" t="str">
@@ -6441,7 +6444,7 @@
     </row>
     <row r="59" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C59" t="str">
-        <f>IFERROR(LOOKUP($B59,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B59,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E59" t="str">
@@ -6455,7 +6458,7 @@
     </row>
     <row r="60" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C60" t="str">
-        <f>IFERROR(LOOKUP($B60,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B60,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E60" t="str">
@@ -6469,7 +6472,7 @@
     </row>
     <row r="61" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C61" t="str">
-        <f>IFERROR(LOOKUP($B61,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B61,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E61" t="str">
@@ -6483,7 +6486,7 @@
     </row>
     <row r="62" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C62" t="str">
-        <f>IFERROR(LOOKUP($B62,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B62,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E62" t="str">
@@ -6497,7 +6500,7 @@
     </row>
     <row r="63" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C63" t="str">
-        <f>IFERROR(LOOKUP($B63,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B63,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E63" t="str">
@@ -6511,7 +6514,7 @@
     </row>
     <row r="64" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C64" t="str">
-        <f>IFERROR(LOOKUP($B64,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B64,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E64" t="str">
@@ -6525,7 +6528,7 @@
     </row>
     <row r="65" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C65" t="str">
-        <f>IFERROR(LOOKUP($B65,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B65,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E65" t="str">
@@ -6539,7 +6542,7 @@
     </row>
     <row r="66" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C66" t="str">
-        <f>IFERROR(LOOKUP($B66,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B66,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E66" t="str">
@@ -6553,7 +6556,7 @@
     </row>
     <row r="67" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C67" t="str">
-        <f>IFERROR(LOOKUP($B67,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B67,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E67" t="str">
@@ -6567,7 +6570,7 @@
     </row>
     <row r="68" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C68" t="str">
-        <f>IFERROR(LOOKUP($B68,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B68,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E68" t="str">
@@ -6581,7 +6584,7 @@
     </row>
     <row r="69" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C69" t="str">
-        <f>IFERROR(LOOKUP($B69,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B69,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E69" t="str">
@@ -6595,7 +6598,7 @@
     </row>
     <row r="70" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C70" t="str">
-        <f>IFERROR(LOOKUP($B70,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B70,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E70" t="str">
@@ -6609,7 +6612,7 @@
     </row>
     <row r="71" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C71" t="str">
-        <f>IFERROR(LOOKUP($B71,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B71,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E71" t="str">
@@ -6623,7 +6626,7 @@
     </row>
     <row r="72" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C72" t="str">
-        <f>IFERROR(LOOKUP($B72,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B72,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E72" t="str">
@@ -6637,7 +6640,7 @@
     </row>
     <row r="73" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C73" t="str">
-        <f>IFERROR(LOOKUP($B73,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B73,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E73" t="str">
@@ -6651,7 +6654,7 @@
     </row>
     <row r="74" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C74" t="str">
-        <f>IFERROR(LOOKUP($B74,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B74,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E74" t="str">
@@ -6665,7 +6668,7 @@
     </row>
     <row r="75" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C75" t="str">
-        <f>IFERROR(LOOKUP($B75,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B75,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E75" t="str">
@@ -6679,7 +6682,7 @@
     </row>
     <row r="76" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C76" t="str">
-        <f>IFERROR(LOOKUP($B76,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B76,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E76" t="str">
@@ -6693,7 +6696,7 @@
     </row>
     <row r="77" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C77" t="str">
-        <f>IFERROR(LOOKUP($B77,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B77,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E77" t="str">
@@ -6707,7 +6710,7 @@
     </row>
     <row r="78" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C78" t="str">
-        <f>IFERROR(LOOKUP($B78,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B78,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E78" t="str">
@@ -6721,7 +6724,7 @@
     </row>
     <row r="79" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C79" t="str">
-        <f>IFERROR(LOOKUP($B79,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B79,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E79" t="str">
@@ -6735,7 +6738,7 @@
     </row>
     <row r="80" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C80" t="str">
-        <f>IFERROR(LOOKUP($B80,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B80,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E80" t="str">
@@ -6749,7 +6752,7 @@
     </row>
     <row r="81" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C81" t="str">
-        <f>IFERROR(LOOKUP($B81,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B81,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E81" t="str">
@@ -6763,7 +6766,7 @@
     </row>
     <row r="82" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C82" t="str">
-        <f>IFERROR(LOOKUP($B82,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B82,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E82" t="str">
@@ -6777,7 +6780,7 @@
     </row>
     <row r="83" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C83" t="str">
-        <f>IFERROR(LOOKUP($B83,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B83,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E83" t="str">
@@ -6791,7 +6794,7 @@
     </row>
     <row r="84" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C84" t="str">
-        <f>IFERROR(LOOKUP($B84,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B84,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E84" t="str">
@@ -6805,7 +6808,7 @@
     </row>
     <row r="85" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C85" t="str">
-        <f>IFERROR(LOOKUP($B85,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B85,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E85" t="str">
@@ -6819,7 +6822,7 @@
     </row>
     <row r="86" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C86" t="str">
-        <f>IFERROR(LOOKUP($B86,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B86,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E86" t="str">
@@ -6833,7 +6836,7 @@
     </row>
     <row r="87" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C87" t="str">
-        <f>IFERROR(LOOKUP($B87,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B87,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E87" t="str">
@@ -6847,7 +6850,7 @@
     </row>
     <row r="88" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C88" t="str">
-        <f>IFERROR(LOOKUP($B88,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B88,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E88" t="str">
@@ -6861,7 +6864,7 @@
     </row>
     <row r="89" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C89" t="str">
-        <f>IFERROR(LOOKUP($B89,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B89,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E89" t="str">
@@ -6875,7 +6878,7 @@
     </row>
     <row r="90" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C90" t="str">
-        <f>IFERROR(LOOKUP($B90,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B90,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E90" t="str">
@@ -6889,7 +6892,7 @@
     </row>
     <row r="91" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C91" t="str">
-        <f>IFERROR(LOOKUP($B91,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B91,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E91" t="str">
@@ -6903,7 +6906,7 @@
     </row>
     <row r="92" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C92" t="str">
-        <f>IFERROR(LOOKUP($B92,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B92,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E92" t="str">
@@ -6917,7 +6920,7 @@
     </row>
     <row r="93" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C93" t="str">
-        <f>IFERROR(LOOKUP($B93,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B93,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E93" t="str">
@@ -6931,7 +6934,7 @@
     </row>
     <row r="94" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C94" t="str">
-        <f>IFERROR(LOOKUP($B94,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B94,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E94" t="str">
@@ -6945,7 +6948,7 @@
     </row>
     <row r="95" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C95" t="str">
-        <f>IFERROR(LOOKUP($B95,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B95,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E95" t="str">
@@ -6959,7 +6962,7 @@
     </row>
     <row r="96" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C96" t="str">
-        <f>IFERROR(LOOKUP($B96,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B96,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E96" t="str">
@@ -6973,7 +6976,7 @@
     </row>
     <row r="97" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C97" t="str">
-        <f>IFERROR(LOOKUP($B97,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B97,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E97" t="str">
@@ -6987,7 +6990,7 @@
     </row>
     <row r="98" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C98" t="str">
-        <f>IFERROR(LOOKUP($B98,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B98,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E98" t="str">
@@ -7001,7 +7004,7 @@
     </row>
     <row r="99" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C99" t="str">
-        <f>IFERROR(LOOKUP($B99,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B99,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E99" t="str">
@@ -7015,7 +7018,7 @@
     </row>
     <row r="100" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C100" t="str">
-        <f>IFERROR(LOOKUP($B100,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B100,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E100" t="str">
@@ -7029,7 +7032,7 @@
     </row>
     <row r="101" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C101" t="str">
-        <f>IFERROR(LOOKUP($B101,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B101,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E101" t="str">
@@ -7043,7 +7046,7 @@
     </row>
     <row r="102" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C102" t="str">
-        <f>IFERROR(LOOKUP($B102,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B102,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E102" t="str">
@@ -7057,7 +7060,7 @@
     </row>
     <row r="103" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C103" t="str">
-        <f>IFERROR(LOOKUP($B103,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B103,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E103" t="str">
@@ -7071,7 +7074,7 @@
     </row>
     <row r="104" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C104" t="str">
-        <f>IFERROR(LOOKUP($B104,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B104,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E104" t="str">
@@ -7085,7 +7088,7 @@
     </row>
     <row r="105" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C105" t="str">
-        <f>IFERROR(LOOKUP($B105,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B105,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E105" t="str">
@@ -7099,7 +7102,7 @@
     </row>
     <row r="106" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C106" t="str">
-        <f>IFERROR(LOOKUP($B106,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B106,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E106" t="str">
@@ -7113,7 +7116,7 @@
     </row>
     <row r="107" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C107" t="str">
-        <f>IFERROR(LOOKUP($B107,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B107,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E107" t="str">
@@ -7127,7 +7130,7 @@
     </row>
     <row r="108" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C108" t="str">
-        <f>IFERROR(LOOKUP($B108,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B108,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E108" t="str">
@@ -7141,7 +7144,7 @@
     </row>
     <row r="109" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C109" t="str">
-        <f>IFERROR(LOOKUP($B109,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B109,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E109" t="str">
@@ -7155,7 +7158,7 @@
     </row>
     <row r="110" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C110" t="str">
-        <f>IFERROR(LOOKUP($B110,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B110,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E110" t="str">
@@ -7169,7 +7172,7 @@
     </row>
     <row r="111" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C111" t="str">
-        <f>IFERROR(LOOKUP($B111,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B111,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E111" t="str">
@@ -7183,7 +7186,7 @@
     </row>
     <row r="112" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C112" t="str">
-        <f>IFERROR(LOOKUP($B112,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B112,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E112" t="str">
@@ -7197,7 +7200,7 @@
     </row>
     <row r="113" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C113" t="str">
-        <f>IFERROR(LOOKUP($B113,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B113,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E113" t="str">
@@ -7211,7 +7214,7 @@
     </row>
     <row r="114" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C114" t="str">
-        <f>IFERROR(LOOKUP($B114,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B114,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E114" t="str">
@@ -7225,7 +7228,7 @@
     </row>
     <row r="115" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C115" t="str">
-        <f>IFERROR(LOOKUP($B115,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B115,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E115" t="str">
@@ -7239,7 +7242,7 @@
     </row>
     <row r="116" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C116" t="str">
-        <f>IFERROR(LOOKUP($B116,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B116,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E116" t="str">
@@ -7253,7 +7256,7 @@
     </row>
     <row r="117" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C117" t="str">
-        <f>IFERROR(LOOKUP($B117,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B117,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E117" t="str">
@@ -7267,7 +7270,7 @@
     </row>
     <row r="118" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C118" t="str">
-        <f>IFERROR(LOOKUP($B118,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B118,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E118" t="str">
@@ -7281,7 +7284,7 @@
     </row>
     <row r="119" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C119" t="str">
-        <f>IFERROR(LOOKUP($B119,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B119,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E119" t="str">
@@ -7295,7 +7298,7 @@
     </row>
     <row r="120" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C120" t="str">
-        <f>IFERROR(LOOKUP($B120,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B120,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E120" t="str">
@@ -7309,7 +7312,7 @@
     </row>
     <row r="121" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C121" t="str">
-        <f>IFERROR(LOOKUP($B121,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B121,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E121" t="str">
@@ -7323,7 +7326,7 @@
     </row>
     <row r="122" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C122" t="str">
-        <f>IFERROR(LOOKUP($B122,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B122,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E122" t="str">
@@ -7337,7 +7340,7 @@
     </row>
     <row r="123" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C123" t="str">
-        <f>IFERROR(LOOKUP($B123,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B123,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E123" t="str">
@@ -7351,7 +7354,7 @@
     </row>
     <row r="124" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C124" t="str">
-        <f>IFERROR(LOOKUP($B124,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B124,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E124" t="str">
@@ -7365,7 +7368,7 @@
     </row>
     <row r="125" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C125" t="str">
-        <f>IFERROR(LOOKUP($B125,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B125,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E125" t="str">
@@ -7379,7 +7382,7 @@
     </row>
     <row r="126" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C126" t="str">
-        <f>IFERROR(LOOKUP($B126,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B126,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E126" t="str">
@@ -7393,7 +7396,7 @@
     </row>
     <row r="127" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C127" t="str">
-        <f>IFERROR(LOOKUP($B127,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B127,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E127" t="str">
@@ -7407,7 +7410,7 @@
     </row>
     <row r="128" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C128" t="str">
-        <f>IFERROR(LOOKUP($B128,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B128,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E128" t="str">
@@ -7421,7 +7424,7 @@
     </row>
     <row r="129" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C129" t="str">
-        <f>IFERROR(LOOKUP($B129,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B129,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E129" t="str">
@@ -7435,7 +7438,7 @@
     </row>
     <row r="130" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C130" t="str">
-        <f>IFERROR(LOOKUP($B130,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B130,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E130" t="str">
@@ -7449,7 +7452,7 @@
     </row>
     <row r="131" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C131" t="str">
-        <f>IFERROR(LOOKUP($B131,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B131,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E131" t="str">
@@ -7463,7 +7466,7 @@
     </row>
     <row r="132" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C132" t="str">
-        <f>IFERROR(LOOKUP($B132,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B132,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E132" t="str">
@@ -7477,7 +7480,7 @@
     </row>
     <row r="133" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C133" t="str">
-        <f>IFERROR(LOOKUP($B133,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B133,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E133" t="str">
@@ -7491,7 +7494,7 @@
     </row>
     <row r="134" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C134" t="str">
-        <f>IFERROR(LOOKUP($B134,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B134,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E134" t="str">
@@ -7505,7 +7508,7 @@
     </row>
     <row r="135" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C135" t="str">
-        <f>IFERROR(LOOKUP($B135,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B135,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E135" t="str">
@@ -7519,7 +7522,7 @@
     </row>
     <row r="136" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C136" t="str">
-        <f>IFERROR(LOOKUP($B136,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B136,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E136" t="str">
@@ -7533,7 +7536,7 @@
     </row>
     <row r="137" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C137" t="str">
-        <f>IFERROR(LOOKUP($B137,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B137,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E137" t="str">
@@ -7547,7 +7550,7 @@
     </row>
     <row r="138" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C138" t="str">
-        <f>IFERROR(LOOKUP($B138,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B138,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E138" t="str">
@@ -7561,7 +7564,7 @@
     </row>
     <row r="139" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C139" t="str">
-        <f>IFERROR(LOOKUP($B139,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B139,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E139" t="str">
@@ -7575,7 +7578,7 @@
     </row>
     <row r="140" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C140" t="str">
-        <f>IFERROR(LOOKUP($B140,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B140,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E140" t="str">
@@ -7589,7 +7592,7 @@
     </row>
     <row r="141" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C141" t="str">
-        <f>IFERROR(LOOKUP($B141,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B141,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E141" t="str">
@@ -7603,7 +7606,7 @@
     </row>
     <row r="142" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C142" t="str">
-        <f>IFERROR(LOOKUP($B142,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B142,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E142" t="str">
@@ -7617,7 +7620,7 @@
     </row>
     <row r="143" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C143" t="str">
-        <f>IFERROR(LOOKUP($B143,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B143,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E143" t="str">
@@ -7631,7 +7634,7 @@
     </row>
     <row r="144" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C144" t="str">
-        <f>IFERROR(LOOKUP($B144,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B144,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E144" t="str">
@@ -7645,7 +7648,7 @@
     </row>
     <row r="145" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C145" t="str">
-        <f>IFERROR(LOOKUP($B145,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B145,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E145" t="str">
@@ -7659,7 +7662,7 @@
     </row>
     <row r="146" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C146" t="str">
-        <f>IFERROR(LOOKUP($B146,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B146,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E146" t="str">
@@ -7673,7 +7676,7 @@
     </row>
     <row r="147" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C147" t="str">
-        <f>IFERROR(LOOKUP($B147,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B147,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E147" t="str">
@@ -7687,7 +7690,7 @@
     </row>
     <row r="148" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C148" t="str">
-        <f>IFERROR(LOOKUP($B148,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B148,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E148" t="str">
@@ -7701,7 +7704,7 @@
     </row>
     <row r="149" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C149" t="str">
-        <f>IFERROR(LOOKUP($B149,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B149,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E149" t="str">
@@ -7715,7 +7718,7 @@
     </row>
     <row r="150" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C150" t="str">
-        <f>IFERROR(LOOKUP($B150,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B150,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E150" t="str">
@@ -7729,7 +7732,7 @@
     </row>
     <row r="151" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C151" t="str">
-        <f>IFERROR(LOOKUP($B151,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B151,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E151" t="str">
@@ -7743,7 +7746,7 @@
     </row>
     <row r="152" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C152" t="str">
-        <f>IFERROR(LOOKUP($B152,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B152,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E152" t="str">
@@ -7757,7 +7760,7 @@
     </row>
     <row r="153" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C153" t="str">
-        <f>IFERROR(LOOKUP($B153,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B153,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E153" t="str">
@@ -7771,7 +7774,7 @@
     </row>
     <row r="154" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C154" t="str">
-        <f>IFERROR(LOOKUP($B154,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B154,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E154" t="str">
@@ -7785,7 +7788,7 @@
     </row>
     <row r="155" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C155" t="str">
-        <f>IFERROR(LOOKUP($B155,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B155,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E155" t="str">
@@ -7799,7 +7802,7 @@
     </row>
     <row r="156" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C156" t="str">
-        <f>IFERROR(LOOKUP($B156,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B156,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E156" t="str">
@@ -7813,7 +7816,7 @@
     </row>
     <row r="157" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C157" t="str">
-        <f>IFERROR(LOOKUP($B157,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B157,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E157" t="str">
@@ -7827,7 +7830,7 @@
     </row>
     <row r="158" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C158" t="str">
-        <f>IFERROR(LOOKUP($B158,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B158,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E158" t="str">
@@ -7841,7 +7844,7 @@
     </row>
     <row r="159" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C159" t="str">
-        <f>IFERROR(LOOKUP($B159,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B159,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E159" t="str">
@@ -7855,7 +7858,7 @@
     </row>
     <row r="160" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C160" t="str">
-        <f>IFERROR(LOOKUP($B160,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B160,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E160" t="str">
@@ -7869,7 +7872,7 @@
     </row>
     <row r="161" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C161" t="str">
-        <f>IFERROR(LOOKUP($B161,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B161,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E161" t="str">
@@ -7883,7 +7886,7 @@
     </row>
     <row r="162" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C162" t="str">
-        <f>IFERROR(LOOKUP($B162,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B162,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E162" t="str">
@@ -7897,7 +7900,7 @@
     </row>
     <row r="163" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C163" t="str">
-        <f>IFERROR(LOOKUP($B163,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B163,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E163" t="str">
@@ -7911,7 +7914,7 @@
     </row>
     <row r="164" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C164" t="str">
-        <f>IFERROR(LOOKUP($B164,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B164,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E164" t="str">
@@ -7925,7 +7928,7 @@
     </row>
     <row r="165" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C165" t="str">
-        <f>IFERROR(LOOKUP($B165,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B165,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E165" t="str">
@@ -7939,7 +7942,7 @@
     </row>
     <row r="166" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C166" t="str">
-        <f>IFERROR(LOOKUP($B166,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B166,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E166" t="str">
@@ -7953,7 +7956,7 @@
     </row>
     <row r="167" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C167" t="str">
-        <f>IFERROR(LOOKUP($B167,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B167,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E167" t="str">
@@ -7967,7 +7970,7 @@
     </row>
     <row r="168" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C168" t="str">
-        <f>IFERROR(LOOKUP($B168,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B168,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E168" t="str">
@@ -7981,7 +7984,7 @@
     </row>
     <row r="169" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C169" t="str">
-        <f>IFERROR(LOOKUP($B169,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B169,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E169" t="str">
@@ -7995,7 +7998,7 @@
     </row>
     <row r="170" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C170" t="str">
-        <f>IFERROR(LOOKUP($B170,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B170,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E170" t="str">
@@ -8009,7 +8012,7 @@
     </row>
     <row r="171" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C171" t="str">
-        <f>IFERROR(LOOKUP($B171,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B171,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E171" t="str">
@@ -8023,7 +8026,7 @@
     </row>
     <row r="172" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C172" t="str">
-        <f>IFERROR(LOOKUP($B172,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B172,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E172" t="str">
@@ -8037,7 +8040,7 @@
     </row>
     <row r="173" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C173" t="str">
-        <f>IFERROR(LOOKUP($B173,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B173,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E173" t="str">
@@ -8051,7 +8054,7 @@
     </row>
     <row r="174" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C174" t="str">
-        <f>IFERROR(LOOKUP($B174,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B174,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E174" t="str">
@@ -8065,7 +8068,7 @@
     </row>
     <row r="175" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C175" t="str">
-        <f>IFERROR(LOOKUP($B175,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B175,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E175" t="str">
@@ -8079,7 +8082,7 @@
     </row>
     <row r="176" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C176" t="str">
-        <f>IFERROR(LOOKUP($B176,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B176,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E176" t="str">
@@ -8093,7 +8096,7 @@
     </row>
     <row r="177" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C177" t="str">
-        <f>IFERROR(LOOKUP($B177,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B177,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E177" t="str">
@@ -8107,7 +8110,7 @@
     </row>
     <row r="178" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C178" t="str">
-        <f>IFERROR(LOOKUP($B178,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B178,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E178" t="str">
@@ -8121,7 +8124,7 @@
     </row>
     <row r="179" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C179" t="str">
-        <f>IFERROR(LOOKUP($B179,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B179,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E179" t="str">
@@ -8135,7 +8138,7 @@
     </row>
     <row r="180" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C180" t="str">
-        <f>IFERROR(LOOKUP($B180,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B180,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E180" t="str">
@@ -8149,7 +8152,7 @@
     </row>
     <row r="181" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C181" t="str">
-        <f>IFERROR(LOOKUP($B181,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B181,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E181" t="str">
@@ -8163,7 +8166,7 @@
     </row>
     <row r="182" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C182" t="str">
-        <f>IFERROR(LOOKUP($B182,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B182,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E182" t="str">
@@ -8177,7 +8180,7 @@
     </row>
     <row r="183" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C183" t="str">
-        <f>IFERROR(LOOKUP($B183,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B183,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E183" t="str">
@@ -8191,7 +8194,7 @@
     </row>
     <row r="184" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C184" t="str">
-        <f>IFERROR(LOOKUP($B184,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B184,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E184" t="str">
@@ -8205,7 +8208,7 @@
     </row>
     <row r="185" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C185" t="str">
-        <f>IFERROR(LOOKUP($B185,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B185,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E185" t="str">
@@ -8219,7 +8222,7 @@
     </row>
     <row r="186" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C186" t="str">
-        <f>IFERROR(LOOKUP($B186,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B186,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E186" t="str">
@@ -8233,7 +8236,7 @@
     </row>
     <row r="187" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C187" t="str">
-        <f>IFERROR(LOOKUP($B187,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B187,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E187" t="str">
@@ -8247,7 +8250,7 @@
     </row>
     <row r="188" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C188" t="str">
-        <f>IFERROR(LOOKUP($B188,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B188,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E188" t="str">
@@ -8261,7 +8264,7 @@
     </row>
     <row r="189" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C189" t="str">
-        <f>IFERROR(LOOKUP($B189,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B189,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E189" t="str">
@@ -8275,7 +8278,7 @@
     </row>
     <row r="190" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C190" t="str">
-        <f>IFERROR(LOOKUP($B190,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B190,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E190" t="str">
@@ -8289,7 +8292,7 @@
     </row>
     <row r="191" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C191" t="str">
-        <f>IFERROR(LOOKUP($B191,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B191,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E191" t="str">
@@ -8303,7 +8306,7 @@
     </row>
     <row r="192" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C192" t="str">
-        <f>IFERROR(LOOKUP($B192,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B192,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E192" t="str">
@@ -8317,7 +8320,7 @@
     </row>
     <row r="193" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C193" t="str">
-        <f>IFERROR(LOOKUP($B193,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B193,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E193" t="str">
@@ -8331,7 +8334,7 @@
     </row>
     <row r="194" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C194" t="str">
-        <f>IFERROR(LOOKUP($B194,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B194,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E194" t="str">
@@ -8345,7 +8348,7 @@
     </row>
     <row r="195" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C195" t="str">
-        <f>IFERROR(LOOKUP($B195,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B195,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E195" t="str">
@@ -8359,7 +8362,7 @@
     </row>
     <row r="196" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C196" t="str">
-        <f>IFERROR(LOOKUP($B196,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B196,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E196" t="str">
@@ -8373,7 +8376,7 @@
     </row>
     <row r="197" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C197" t="str">
-        <f>IFERROR(LOOKUP($B197,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B197,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E197" t="str">
@@ -8387,7 +8390,7 @@
     </row>
     <row r="198" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C198" t="str">
-        <f>IFERROR(LOOKUP($B198,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B198,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E198" t="str">
@@ -8401,7 +8404,7 @@
     </row>
     <row r="199" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C199" t="str">
-        <f>IFERROR(LOOKUP($B199,Opiskelijat!$A$3:$A$439,Opiskelijat!$C$3:$C$439),"")</f>
+        <f>IFERROR(LOOKUP($B199,Opiskelijat!$A$3:$A$2221,Opiskelijat!$B$3:$B$2221),"")</f>
         <v/>
       </c>
       <c r="E199" t="str">
@@ -8633,7 +8636,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tutkinnot!$A$3:$A$438</xm:f>
@@ -8644,7 +8647,13 @@
           <x14:formula1>
             <xm:f>Opiskelijat!$A$3:$A$20</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B218</xm:sqref>
+          <xm:sqref>B200:B218</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Opiskelijat!$A$3:$A$2221</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5:B199</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -20106,8 +20115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20117,7 +20126,7 @@
         <v>1243</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>1689</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1240</v>

</xml_diff>